<commit_message>
journal final + use cases final + fixes tablePoints
</commit_message>
<xml_diff>
--- a/Documentation/Annexes/Journal de travail_MB.xlsx
+++ b/Documentation/Annexes/Journal de travail_MB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\Shoot4Stats\Documentation\Rendu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\Shoot4Stats\Documentation\Annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$89</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$B$1:$G$95</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="83">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -255,6 +255,27 @@
   </si>
   <si>
     <t>Petites stylisations afin de rendre l'appli nette</t>
+  </si>
+  <si>
+    <t>Mise en place d'un selecteur fait maisn pour les points</t>
+  </si>
+  <si>
+    <t>Mise en place d'un tableau dynamique si nb de flèches &gt;  6</t>
+  </si>
+  <si>
+    <t>Fix de quelques bugs mineurs rapportés par les testeurs</t>
+  </si>
+  <si>
+    <t>Rédaction / finitions du rapport</t>
+  </si>
+  <si>
+    <t>Impression du rapport et relecture et impression des Annexes</t>
+  </si>
+  <si>
+    <t>Envoi mail + début rédaction Bref rapport TPI</t>
+  </si>
+  <si>
+    <t>Reliure du dossier et envoi dossier courier A Poste après relcture et vérifications</t>
   </si>
 </sst>
 </file>
@@ -489,7 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -709,9 +730,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1003,10 +1021,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K90"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1061,10 +1082,6 @@
       <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="74" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1080,13 +1097,6 @@
       <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="48">
-        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E85,E89,E35,E68,E78)*24</f>
-        <v>93.149999999999991</v>
-      </c>
-      <c r="I5" s="45" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
@@ -1239,11 +1249,11 @@
       <c r="B16" s="66">
         <v>42824</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="77"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="76"/>
       <c r="F16" s="10" t="s">
         <v>12</v>
       </c>
@@ -2202,7 +2212,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="27">
         <v>0.5</v>
@@ -2217,7 +2227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="27">
         <v>0.58333333333333337</v>
@@ -2232,7 +2242,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="27">
         <v>0.625</v>
@@ -2247,7 +2257,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="9"/>
       <c r="C84" s="27">
         <v>0.65625</v>
@@ -2262,7 +2272,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="32" t="s">
         <v>4</v>
@@ -2274,56 +2284,152 @@
       </c>
       <c r="F85" s="55"/>
     </row>
-    <row r="86" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="7">
         <v>42843</v>
       </c>
-      <c r="C86" s="16"/>
-      <c r="D86" s="57"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="59"/>
-    </row>
-    <row r="87" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D86" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F86" s="59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="15"/>
-      <c r="F87" s="60"/>
-    </row>
-    <row r="88" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="17">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D87" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="15">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F87" s="60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="60"/>
-    </row>
-    <row r="89" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="63"/>
-      <c r="B89" s="62"/>
-      <c r="C89" s="42" t="s">
+      <c r="C88" s="17">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D88" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F88" s="60" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="C89" s="17">
+        <v>0.53125</v>
+      </c>
+      <c r="D89" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E89" s="15">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F89" s="60" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="5"/>
+      <c r="C90" s="17">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D90" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" s="15">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F90" s="60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="C91" s="17">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D91" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" s="15">
+        <v>0.6875</v>
+      </c>
+      <c r="F91" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="C92" s="19">
+        <v>0.6875</v>
+      </c>
+      <c r="D92" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" s="15">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="F92" s="60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="63"/>
+      <c r="B93" s="62"/>
+      <c r="C93" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D89" s="42"/>
-      <c r="E89" s="64">
-        <f>E88-C88+E87-C87+E86-C86</f>
-        <v>0</v>
-      </c>
-      <c r="F89" s="61"/>
-    </row>
-    <row r="90" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="24"/>
-      <c r="C90" s="57"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="64">
+        <f>E91-C91+E87-C87+E86-C86+E88-C88+E89-C89+E90-C90+E92-C92</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F93" s="61"/>
+    </row>
+    <row r="94" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="24"/>
+      <c r="C94" s="57"/>
+      <c r="F94" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G94" s="45"/>
+    </row>
+    <row r="95" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F95" s="48">
+        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E85,E93,E35,E68,E78)*24</f>
+        <v>101.54999999999998</v>
+      </c>
+      <c r="G95" s="45" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>